<commit_message>
Update reduced coeffs and shifts of Ne TDHF
</commit_message>
<xml_diff>
--- a/Data/Simulated Ne beta parameters, TDHF, 2018-09-17.xlsx
+++ b/Data/Simulated Ne beta parameters, TDHF, 2018-09-17.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daehyun/Documents/FERMI 20144077 Ueda/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1435A92-93F1-3140-B21C-D16ADDEBE17A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05157CBA-BD6A-9149-B045-7CDD5B6C42C5}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35920" yWindow="460" windowWidth="25560" windowHeight="18880" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38580" yWindow="1520" windowWidth="25560" windowHeight="18880" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="w2w" sheetId="18" r:id="rId1"/>
-    <sheet name="wonly" sheetId="11" r:id="rId2"/>
-    <sheet name="good1" sheetId="12" r:id="rId3"/>
-    <sheet name="good2" sheetId="13" r:id="rId4"/>
-    <sheet name="good3" sheetId="14" r:id="rId5"/>
-    <sheet name="good4" sheetId="15" r:id="rId6"/>
-    <sheet name="k" sheetId="16" r:id="rId7"/>
+    <sheet name="w2w_fitted" sheetId="20" r:id="rId2"/>
+    <sheet name="wonly" sheetId="11" r:id="rId3"/>
+    <sheet name="Reduced" sheetId="19" r:id="rId4"/>
+    <sheet name="good1" sheetId="12" r:id="rId5"/>
+    <sheet name="good2" sheetId="13" r:id="rId6"/>
+    <sheet name="good3" sheetId="14" r:id="rId7"/>
+    <sheet name="good4" sheetId="15" r:id="rId8"/>
+    <sheet name="k" sheetId="16" r:id="rId9"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="39">
   <si>
     <t>beta1</t>
   </si>
@@ -51,9 +53,6 @@
     <t>phi (deg)</t>
   </si>
   <si>
-    <t>photon (eV)</t>
-  </si>
-  <si>
     <t>good1</t>
   </si>
   <si>
@@ -75,9 +74,6 @@
     <t>p_amp</t>
   </si>
   <si>
-    <t>p_arg</t>
-  </si>
-  <si>
     <t>sp_amp</t>
   </si>
   <si>
@@ -87,32 +83,87 @@
     <t>fdp_amp</t>
   </si>
   <si>
-    <t>sp_arg</t>
-  </si>
-  <si>
-    <t>dp_arg</t>
-  </si>
-  <si>
-    <t>fdp_arg</t>
-  </si>
-  <si>
     <t>psp_amp</t>
   </si>
   <si>
     <t>pdp_amp</t>
   </si>
   <si>
-    <t>target dataset</t>
+    <t>fdp_shift</t>
+  </si>
+  <si>
+    <t>sp_shift</t>
+  </si>
+  <si>
+    <t>p_shift</t>
+  </si>
+  <si>
+    <t>dp_shift</t>
+  </si>
+  <si>
+    <t>coeff_dp</t>
+  </si>
+  <si>
+    <t>coeff_sp</t>
+  </si>
+  <si>
+    <t>coeff_psp</t>
+  </si>
+  <si>
+    <t>coeff_pdp</t>
+  </si>
+  <si>
+    <t>coeff_fdp</t>
+  </si>
+  <si>
+    <t>eta_sp</t>
+  </si>
+  <si>
+    <t>eta_psp</t>
+  </si>
+  <si>
+    <t>eta_pdp</t>
+  </si>
+  <si>
+    <t>eta_dp</t>
+  </si>
+  <si>
+    <t>eta_fdp</t>
+  </si>
+  <si>
+    <t>Target dataset</t>
+  </si>
+  <si>
+    <t>Photon (eV)</t>
+  </si>
+  <si>
+    <t>beta1_amp</t>
+  </si>
+  <si>
+    <t>beta1_shift</t>
+  </si>
+  <si>
+    <t>beta3_amp</t>
+  </si>
+  <si>
+    <t>beta3_shift</t>
+  </si>
+  <si>
+    <t>beta1m3_amp</t>
+  </si>
+  <si>
+    <t>beta1m3_shift</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -150,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -188,11 +239,36 @@
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="68">
+  <dxfs count="87">
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="166" formatCode="0.000"/>
     </dxf>
@@ -824,6 +900,39 @@
       <numFmt numFmtId="166" formatCode="0.000"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="167" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="165" formatCode="0.0000"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -919,20 +1028,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{8778010A-3D1F-DF4F-B2BA-4CD89121205F}" name="Table1311" displayName="Table1311" ref="A1:H33" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{8778010A-3D1F-DF4F-B2BA-4CD89121205F}" name="Table1311" displayName="Table1311" ref="A1:H33" totalsRowShown="0" headerRowDxfId="86" dataDxfId="85">
   <autoFilter ref="A1:H33" xr:uid="{EE0BDB9F-493C-9C4A-8003-F22A7669AAA7}"/>
   <sortState ref="A2:H33">
     <sortCondition ref="A1:A33"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{A9C0E41B-1AFE-674C-90E8-D1D179628E58}" name="target dataset" dataDxfId="65"/>
-    <tableColumn id="2" xr3:uid="{6B63E76C-A142-484A-8040-5F9E2B6ED8BF}" name="photon (eV)" dataDxfId="64"/>
-    <tableColumn id="3" xr3:uid="{C1A5F614-DF39-FE4D-9C68-CF238B7B1FAB}" name="phi (deg)" dataDxfId="63"/>
-    <tableColumn id="4" xr3:uid="{93222719-EACE-D14D-A23C-A29210E3F88D}" name="beta1" dataDxfId="62"/>
-    <tableColumn id="5" xr3:uid="{55463977-50DC-5543-A800-65678C631CA9}" name="beta2" dataDxfId="61"/>
-    <tableColumn id="6" xr3:uid="{A4D18E31-8E47-7540-BFFA-2FF61FA4E199}" name="beta3" dataDxfId="60"/>
-    <tableColumn id="7" xr3:uid="{3032E9A7-5533-1D49-A217-30EF10E5A58C}" name="beta4" dataDxfId="59"/>
-    <tableColumn id="10" xr3:uid="{1466D1E1-9E6B-F34A-A8D5-24AA1175800D}" name="beta1m3" dataDxfId="58">
+    <tableColumn id="1" xr3:uid="{A9C0E41B-1AFE-674C-90E8-D1D179628E58}" name="Target dataset" dataDxfId="84"/>
+    <tableColumn id="2" xr3:uid="{6B63E76C-A142-484A-8040-5F9E2B6ED8BF}" name="Photon (eV)" dataDxfId="83"/>
+    <tableColumn id="3" xr3:uid="{C1A5F614-DF39-FE4D-9C68-CF238B7B1FAB}" name="phi (deg)" dataDxfId="82"/>
+    <tableColumn id="4" xr3:uid="{93222719-EACE-D14D-A23C-A29210E3F88D}" name="beta1" dataDxfId="81"/>
+    <tableColumn id="5" xr3:uid="{55463977-50DC-5543-A800-65678C631CA9}" name="beta2" dataDxfId="80"/>
+    <tableColumn id="6" xr3:uid="{A4D18E31-8E47-7540-BFFA-2FF61FA4E199}" name="beta3" dataDxfId="79"/>
+    <tableColumn id="7" xr3:uid="{3032E9A7-5533-1D49-A217-30EF10E5A58C}" name="beta4" dataDxfId="78"/>
+    <tableColumn id="10" xr3:uid="{1466D1E1-9E6B-F34A-A8D5-24AA1175800D}" name="beta1m3" dataDxfId="77">
       <calculatedColumnFormula>Table1311[[#This Row],[beta1]]-3/2*Table1311[[#This Row],[beta3]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -941,108 +1050,148 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F05A4894-8C70-D642-85C3-3AB7CFBB4F28}" name="Table135" displayName="Table135" ref="A1:E4" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56">
-  <autoFilter ref="A1:E4" xr:uid="{53E4CFBE-4728-384F-AC3E-37B66AF4A439}"/>
-  <sortState ref="A2:E4">
-    <sortCondition ref="A1:A4"/>
-  </sortState>
-  <tableColumns count="5">
-    <tableColumn id="2" xr3:uid="{BD60D2D9-15A2-F545-AAFF-748850E64446}" name="photon (eV)" dataDxfId="55"/>
-    <tableColumn id="4" xr3:uid="{28273152-69FC-A241-BCA6-31BCEA8C2BEC}" name="beta1" dataDxfId="54"/>
-    <tableColumn id="5" xr3:uid="{33E9B38C-ACC9-0A49-9295-DACDF599E7FB}" name="beta2" dataDxfId="53"/>
-    <tableColumn id="6" xr3:uid="{407B9B6B-64D4-014F-A379-342916257ADC}" name="beta3" dataDxfId="52"/>
-    <tableColumn id="7" xr3:uid="{8826E549-F298-AB41-856D-6CC97B08EAB8}" name="beta4" dataDxfId="51"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F2E2C9A5-EA92-964C-82DE-B5A6B7B9B5BE}" name="TDCASSCF" displayName="TDCASSCF" ref="A1:J5" totalsRowShown="0">
+  <autoFilter ref="A1:J5" xr:uid="{FF031212-F70D-1841-B1A7-16ECFE4A851A}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{B583D4BB-9F96-994C-A314-D7FB7341AA8C}" name="Target dataset"/>
+    <tableColumn id="2" xr3:uid="{89667834-04CF-9C4D-9D20-6C00DB34F2BF}" name="Photon (eV)"/>
+    <tableColumn id="15" xr3:uid="{60507A89-BBE8-014A-8D9A-13D578F47D96}" name="beta1_amp" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{7C8D09CD-0B6C-6A41-B1CB-73BD882F1E73}" name="beta1_shift" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{8CCA5178-3667-6640-BC8E-D63DA2EE6D29}" name="beta2" dataDxfId="5"/>
+    <tableColumn id="16" xr3:uid="{485E2375-608B-1A48-96B1-B590DD8C5233}" name="beta3_amp" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{240B768E-BBCE-E944-915A-21D3F550E5B5}" name="beta3_shift" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{DAB6A4F1-E777-2240-BCC5-93E270FEEC6D}" name="beta4" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{8A84BA3D-368F-9D40-B237-2CEAFCB73E75}" name="beta1m3_amp" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{ABBF046B-A08D-394B-BE43-B991E954AD0C}" name="beta1m3_shift" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{59DFE585-94CE-324E-80C4-17D5A8535F3A}" name="Table3" displayName="Table3" ref="A1:I4" totalsRowShown="0" headerRowDxfId="50">
-  <autoFilter ref="A1:I4" xr:uid="{8B5C4BC6-D08A-F342-B69E-95E18573CBD5}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{5BA34F36-7497-CA4F-999F-15736C5C90B3}" name="m" dataDxfId="49"/>
-    <tableColumn id="2" xr3:uid="{A0426779-3323-8542-8FAD-30E204B20D55}" name="sp_amp" dataDxfId="48"/>
-    <tableColumn id="3" xr3:uid="{684B6570-B9E4-704D-8176-FCA5A03A637E}" name="p_amp" dataDxfId="47"/>
-    <tableColumn id="4" xr3:uid="{ADC74BA0-1CC4-1C48-A1F6-685EBC267637}" name="dp_amp" dataDxfId="46"/>
-    <tableColumn id="5" xr3:uid="{2845C546-B0B7-214A-9B3A-94C4A1525E23}" name="fdp_amp" dataDxfId="45"/>
-    <tableColumn id="6" xr3:uid="{1E48FDEC-EE5F-7C46-A4AB-BA8213F216B3}" name="sp_arg" dataDxfId="44"/>
-    <tableColumn id="7" xr3:uid="{CD04CD5C-B6F2-9246-BDA1-EA343D3D5323}" name="p_arg" dataDxfId="43"/>
-    <tableColumn id="8" xr3:uid="{9B5BB2F1-9199-A844-952A-2F3D8A2919AF}" name="dp_arg" dataDxfId="42"/>
-    <tableColumn id="9" xr3:uid="{6B1CD9FD-B8D5-2043-9623-1AE12EBE013F}" name="fdp_arg" dataDxfId="41"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F05A4894-8C70-D642-85C3-3AB7CFBB4F28}" name="Table135" displayName="Table135" ref="A1:E4" totalsRowShown="0" headerRowDxfId="76" dataDxfId="75">
+  <autoFilter ref="A1:E4" xr:uid="{53E4CFBE-4728-384F-AC3E-37B66AF4A439}"/>
+  <sortState ref="A2:E4">
+    <sortCondition ref="A1:A4"/>
+  </sortState>
+  <tableColumns count="5">
+    <tableColumn id="2" xr3:uid="{BD60D2D9-15A2-F545-AAFF-748850E64446}" name="Photon (eV)" dataDxfId="74"/>
+    <tableColumn id="4" xr3:uid="{28273152-69FC-A241-BCA6-31BCEA8C2BEC}" name="beta1" dataDxfId="73"/>
+    <tableColumn id="5" xr3:uid="{33E9B38C-ACC9-0A49-9295-DACDF599E7FB}" name="beta2" dataDxfId="72"/>
+    <tableColumn id="6" xr3:uid="{407B9B6B-64D4-014F-A379-342916257ADC}" name="beta3" dataDxfId="71"/>
+    <tableColumn id="7" xr3:uid="{8826E549-F298-AB41-856D-6CC97B08EAB8}" name="beta4" dataDxfId="70"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{AEAD797E-5610-6742-BF1C-D62A7ADBA7F0}" name="Table5" displayName="Table5" ref="A1:I4" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
-  <autoFilter ref="A1:I4" xr:uid="{B4719746-BFD9-6D4E-8D94-4B12B338165F}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{647D98FB-251B-4542-BF7C-63F898E9AC7E}" name="m" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{2E22E77A-4173-0D4A-9A6F-7E47D1678087}" name="sp_amp" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{D6903029-EBD1-994F-97CC-EBA1ABF4E926}" name="p_amp" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{3DF53176-C13B-7641-82D5-1BE402BDD02F}" name="dp_amp" dataDxfId="35"/>
-    <tableColumn id="5" xr3:uid="{1060BE76-3E32-1A48-9A41-0593EE6FE8C2}" name="fdp_amp" dataDxfId="34"/>
-    <tableColumn id="6" xr3:uid="{FFBFF49F-1059-1642-8A31-AD573823D3E3}" name="sp_arg" dataDxfId="33"/>
-    <tableColumn id="7" xr3:uid="{1D811937-AFDD-8D48-81C8-B33622C03534}" name="p_arg" dataDxfId="32"/>
-    <tableColumn id="8" xr3:uid="{E126B12C-EED2-324A-A8CC-51A76C96BAAD}" name="dp_arg" dataDxfId="31"/>
-    <tableColumn id="9" xr3:uid="{8C65ED6F-4B8F-3246-ABE2-AE3D22B29FF5}" name="fdp_arg" dataDxfId="30"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{648571DC-0017-F44C-9861-5B63C026D27B}" name="Table1" displayName="Table1" ref="A1:L5" totalsRowShown="0">
+  <autoFilter ref="A1:L5" xr:uid="{A6CF40E6-909C-EF45-94C2-61FE41276FD0}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{8EA12F60-3AC0-1B4B-BCF6-65DDE53BE438}" name="Target dataset"/>
+    <tableColumn id="2" xr3:uid="{90E968C9-0904-3A4F-B492-15BEF052B297}" name="Photon (eV)" dataDxfId="69"/>
+    <tableColumn id="3" xr3:uid="{1B597EDE-219E-6241-B37F-8CED0F7B29A1}" name="coeff_sp" dataDxfId="68"/>
+    <tableColumn id="4" xr3:uid="{AA9F4726-D238-224F-9511-86ABE8AC5E51}" name="eta_sp" dataDxfId="67"/>
+    <tableColumn id="5" xr3:uid="{AF5D9ABC-E405-664C-BD87-0CEBF507E41D}" name="coeff_psp" dataDxfId="66"/>
+    <tableColumn id="6" xr3:uid="{64A2F11E-FF0F-A54A-8571-8DCE1875A6D8}" name="eta_psp" dataDxfId="65"/>
+    <tableColumn id="7" xr3:uid="{B475181D-DB43-F347-AC5B-1ADBA027A415}" name="coeff_pdp" dataDxfId="64"/>
+    <tableColumn id="8" xr3:uid="{D74F1B77-0598-E047-BE9E-65FFAA85DFE0}" name="eta_pdp" dataDxfId="63"/>
+    <tableColumn id="9" xr3:uid="{D7428F5C-8F9B-3A4E-BE08-93156A3D8070}" name="coeff_dp" dataDxfId="62"/>
+    <tableColumn id="10" xr3:uid="{219D52DC-F4B2-2846-AE03-BF070C4B6292}" name="eta_dp" dataDxfId="61"/>
+    <tableColumn id="11" xr3:uid="{A8716C4F-8448-6947-98AC-C95A3FA898C7}" name="coeff_fdp" dataDxfId="60"/>
+    <tableColumn id="12" xr3:uid="{C15B8245-F0D7-EB45-8808-6810DC739D05}" name="eta_fdp" dataDxfId="59"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2A026460-1D43-9646-BB18-B4646ACDCF3D}" name="Table6" displayName="Table6" ref="A1:I4" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
-  <autoFilter ref="A1:I4" xr:uid="{A8FC2363-68E6-1D4F-AF75-C41078FEDC29}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{59DFE585-94CE-324E-80C4-17D5A8535F3A}" name="Table3" displayName="Table3" ref="A1:I4" totalsRowShown="0" headerRowDxfId="58">
+  <autoFilter ref="A1:I4" xr:uid="{8B5C4BC6-D08A-F342-B69E-95E18573CBD5}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{67A1216D-8F66-8F47-9DDF-9779C464E009}" name="m" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{7A921D8C-3F15-E140-B838-5A1204B74685}" name="sp_amp" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{F8CDDF88-4BC2-1D4A-84BD-6353BF4B9E77}" name="p_amp" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{1481DC66-2D0E-E04E-B630-3C7741CE4CD0}" name="dp_amp" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{720417F9-6520-2C47-B50F-B0B73F912EED}" name="fdp_amp" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{826D4DF2-FA71-F24E-8ED5-A415C4A6D02B}" name="sp_arg" dataDxfId="22"/>
-    <tableColumn id="7" xr3:uid="{D5972777-E932-ED4A-8B82-9C8059F7E06E}" name="p_arg" dataDxfId="21"/>
-    <tableColumn id="8" xr3:uid="{8DE1440F-E3A9-014F-BD79-E3166B7C3A72}" name="dp_arg" dataDxfId="20"/>
-    <tableColumn id="9" xr3:uid="{19C76EA3-897A-3148-80AE-374F812A5850}" name="fdp_arg" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{5BA34F36-7497-CA4F-999F-15736C5C90B3}" name="m" dataDxfId="57"/>
+    <tableColumn id="2" xr3:uid="{A0426779-3323-8542-8FAD-30E204B20D55}" name="sp_amp" dataDxfId="56"/>
+    <tableColumn id="3" xr3:uid="{684B6570-B9E4-704D-8176-FCA5A03A637E}" name="p_amp" dataDxfId="55"/>
+    <tableColumn id="4" xr3:uid="{ADC74BA0-1CC4-1C48-A1F6-685EBC267637}" name="dp_amp" dataDxfId="54"/>
+    <tableColumn id="5" xr3:uid="{2845C546-B0B7-214A-9B3A-94C4A1525E23}" name="fdp_amp" dataDxfId="53"/>
+    <tableColumn id="6" xr3:uid="{1E48FDEC-EE5F-7C46-A4AB-BA8213F216B3}" name="sp_shift" dataDxfId="52"/>
+    <tableColumn id="7" xr3:uid="{CD04CD5C-B6F2-9246-BDA1-EA343D3D5323}" name="p_shift" dataDxfId="51"/>
+    <tableColumn id="8" xr3:uid="{9B5BB2F1-9199-A844-952A-2F3D8A2919AF}" name="dp_shift" dataDxfId="50"/>
+    <tableColumn id="9" xr3:uid="{6B1CD9FD-B8D5-2043-9623-1AE12EBE013F}" name="fdp_shift" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{E38178F3-1826-3E4D-BBB2-2C0D6EDAE208}" name="Table7" displayName="Table7" ref="A1:I4" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
-  <autoFilter ref="A1:I4" xr:uid="{DC15BAF1-E157-5A42-A33B-060096B22C67}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{AEAD797E-5610-6742-BF1C-D62A7ADBA7F0}" name="Table5" displayName="Table5" ref="A1:I4" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
+  <autoFilter ref="A1:I4" xr:uid="{B4719746-BFD9-6D4E-8D94-4B12B338165F}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{FDE47AB7-D70F-3145-A921-E12C0BE05C94}" name="m" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{D43E9326-FEAF-EE49-A01C-CC943A2F4B91}" name="sp_amp" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{7BDC518E-90F1-4D47-A627-F285D44C0247}" name="p_amp" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{EC03AEAB-910C-CD4C-A25B-38E5F1590E5A}" name="dp_amp" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{608F44B2-D548-C349-A1C6-FE7BFEDBADE8}" name="fdp_amp" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{7E6BAB65-DA36-BC48-B2EB-1A3CFDB0CC8D}" name="sp_arg" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{45305CC1-A33F-8644-8440-E87A9BA944D8}" name="p_arg" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{A4952650-FD28-5B48-8679-6D186F7D7ED6}" name="dp_arg" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{B0FF8D19-EC72-B44F-88D1-021AB69F405F}" name="fdp_arg" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{647D98FB-251B-4542-BF7C-63F898E9AC7E}" name="m" dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{2E22E77A-4173-0D4A-9A6F-7E47D1678087}" name="sp_amp" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{D6903029-EBD1-994F-97CC-EBA1ABF4E926}" name="p_amp" dataDxfId="44"/>
+    <tableColumn id="4" xr3:uid="{3DF53176-C13B-7641-82D5-1BE402BDD02F}" name="dp_amp" dataDxfId="43"/>
+    <tableColumn id="5" xr3:uid="{1060BE76-3E32-1A48-9A41-0593EE6FE8C2}" name="fdp_amp" dataDxfId="42"/>
+    <tableColumn id="6" xr3:uid="{FFBFF49F-1059-1642-8A31-AD573823D3E3}" name="sp_shift" dataDxfId="41"/>
+    <tableColumn id="7" xr3:uid="{1D811937-AFDD-8D48-81C8-B33622C03534}" name="p_shift" dataDxfId="40"/>
+    <tableColumn id="8" xr3:uid="{E126B12C-EED2-324A-A8CC-51A76C96BAAD}" name="dp_shift" dataDxfId="39"/>
+    <tableColumn id="9" xr3:uid="{8C65ED6F-4B8F-3246-ABE2-AE3D22B29FF5}" name="fdp_shift" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{763C1B8E-8E8C-1C43-AF64-24E938897D53}" name="Table19" displayName="Table19" ref="A1:F4" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2A026460-1D43-9646-BB18-B4646ACDCF3D}" name="Table6" displayName="Table6" ref="A1:I4" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
+  <autoFilter ref="A1:I4" xr:uid="{A8FC2363-68E6-1D4F-AF75-C41078FEDC29}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{67A1216D-8F66-8F47-9DDF-9779C464E009}" name="m" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{7A921D8C-3F15-E140-B838-5A1204B74685}" name="sp_amp" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{F8CDDF88-4BC2-1D4A-84BD-6353BF4B9E77}" name="p_amp" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{1481DC66-2D0E-E04E-B630-3C7741CE4CD0}" name="dp_amp" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{720417F9-6520-2C47-B50F-B0B73F912EED}" name="fdp_amp" dataDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{826D4DF2-FA71-F24E-8ED5-A415C4A6D02B}" name="sp_shift" dataDxfId="30"/>
+    <tableColumn id="7" xr3:uid="{D5972777-E932-ED4A-8B82-9C8059F7E06E}" name="p_shift" dataDxfId="29"/>
+    <tableColumn id="8" xr3:uid="{8DE1440F-E3A9-014F-BD79-E3166B7C3A72}" name="dp_shift" dataDxfId="28"/>
+    <tableColumn id="9" xr3:uid="{19C76EA3-897A-3148-80AE-374F812A5850}" name="fdp_shift" dataDxfId="27"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{E38178F3-1826-3E4D-BBB2-2C0D6EDAE208}" name="Table7" displayName="Table7" ref="A1:I4" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+  <autoFilter ref="A1:I4" xr:uid="{DC15BAF1-E157-5A42-A33B-060096B22C67}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{FDE47AB7-D70F-3145-A921-E12C0BE05C94}" name="m" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{D43E9326-FEAF-EE49-A01C-CC943A2F4B91}" name="sp_amp" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{7BDC518E-90F1-4D47-A627-F285D44C0247}" name="p_amp" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{EC03AEAB-910C-CD4C-A25B-38E5F1590E5A}" name="dp_amp" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{608F44B2-D548-C349-A1C6-FE7BFEDBADE8}" name="fdp_amp" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{7E6BAB65-DA36-BC48-B2EB-1A3CFDB0CC8D}" name="sp_shift" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{45305CC1-A33F-8644-8440-E87A9BA944D8}" name="p_shift" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{A4952650-FD28-5B48-8679-6D186F7D7ED6}" name="dp_shift" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{B0FF8D19-EC72-B44F-88D1-021AB69F405F}" name="fdp_shift" dataDxfId="16"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{763C1B8E-8E8C-1C43-AF64-24E938897D53}" name="Table19" displayName="Table19" ref="A1:F4" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A1:F4" xr:uid="{B629EAAC-C030-3144-A5C8-EA87A0850D51}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{678C78C9-26BE-E640-8E8C-8BD4C90EA1D8}" name="m" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{F4BE6F06-FE79-854C-A751-08C0116B4DA2}" name="sp_amp" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{5D349974-DB77-004C-A546-3F935BF8CE78}" name="psp_amp" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{914971F8-D9D5-3042-9BBD-39AA14A4A973}" name="pdp_amp" dataDxfId="2">
+    <tableColumn id="1" xr3:uid="{678C78C9-26BE-E640-8E8C-8BD4C90EA1D8}" name="m" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{F4BE6F06-FE79-854C-A751-08C0116B4DA2}" name="sp_amp" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{5D349974-DB77-004C-A546-3F935BF8CE78}" name="psp_amp" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{914971F8-D9D5-3042-9BBD-39AA14A4A973}" name="pdp_amp" dataDxfId="10">
       <calculatedColumnFormula>-SQRT(15)/10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{1E5B610A-F2B0-C845-8B12-F74BAEE6BEAC}" name="dp_amp" dataDxfId="1">
-      <calculatedColumnFormula>SQRT(2)/2</calculatedColumnFormula>
+    <tableColumn id="5" xr3:uid="{1E5B610A-F2B0-C845-8B12-F74BAEE6BEAC}" name="dp_amp" dataDxfId="9">
+      <calculatedColumnFormula>SQRT(30)/15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9597E78F-47B1-1F45-BC2F-077AD7E519D2}" name="fdp_amp" dataDxfId="0">
+    <tableColumn id="6" xr3:uid="{9597E78F-47B1-1F45-BC2F-077AD7E519D2}" name="fdp_amp" dataDxfId="8">
       <calculatedColumnFormula>2*SQRT(15)/15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1316,12 +1465,12 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="8.33203125" style="14" bestFit="1" customWidth="1"/>
@@ -1330,10 +1479,10 @@
   <sheetData>
     <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>4</v>
@@ -1351,12 +1500,12 @@
         <v>3</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="12">
         <v>15.9</v>
@@ -1383,7 +1532,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="12">
         <v>15.9</v>
@@ -1410,7 +1559,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="12">
         <v>15.9</v>
@@ -1437,7 +1586,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="12">
         <v>15.9</v>
@@ -1464,7 +1613,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="12">
         <v>15.9</v>
@@ -1491,7 +1640,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="12">
         <v>15.9</v>
@@ -1518,7 +1667,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="12">
         <v>15.9</v>
@@ -1545,7 +1694,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="12">
         <v>15.9</v>
@@ -1572,7 +1721,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="12">
         <v>14.3</v>
@@ -1599,7 +1748,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" s="12">
         <v>14.3</v>
@@ -1626,7 +1775,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" s="12">
         <v>14.3</v>
@@ -1653,7 +1802,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" s="12">
         <v>14.3</v>
@@ -1680,7 +1829,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" s="12">
         <v>14.3</v>
@@ -1707,7 +1856,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B15" s="12">
         <v>14.3</v>
@@ -1734,7 +1883,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16" s="12">
         <v>14.3</v>
@@ -1761,7 +1910,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B17" s="12">
         <v>14.3</v>
@@ -1788,7 +1937,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B18" s="12">
         <v>19.100000000000001</v>
@@ -1815,7 +1964,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B19" s="12">
         <v>19.100000000000001</v>
@@ -1842,7 +1991,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B20" s="12">
         <v>19.100000000000001</v>
@@ -1869,7 +2018,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B21" s="12">
         <v>19.100000000000001</v>
@@ -1896,7 +2045,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B22" s="12">
         <v>19.100000000000001</v>
@@ -1923,7 +2072,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B23" s="12">
         <v>19.100000000000001</v>
@@ -1950,7 +2099,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B24" s="12">
         <v>19.100000000000001</v>
@@ -1977,7 +2126,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B25" s="12">
         <v>19.100000000000001</v>
@@ -2004,7 +2153,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B26" s="12">
         <v>15.9</v>
@@ -2031,7 +2180,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B27" s="12">
         <v>15.9</v>
@@ -2058,7 +2207,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B28" s="12">
         <v>15.9</v>
@@ -2085,7 +2234,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B29" s="12">
         <v>15.9</v>
@@ -2112,7 +2261,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B30" s="12">
         <v>15.9</v>
@@ -2139,7 +2288,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B31" s="12">
         <v>15.9</v>
@@ -2166,7 +2315,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B32" s="12">
         <v>15.9</v>
@@ -2193,7 +2342,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B33" s="12">
         <v>15.9</v>
@@ -2227,11 +2376,198 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1CACF38-0506-9A43-8C40-38E5FAC9927C}">
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>15.9</v>
+      </c>
+      <c r="C2" s="14">
+        <v>0.75980258000000001</v>
+      </c>
+      <c r="D2" s="14">
+        <v>1.5804219100000001</v>
+      </c>
+      <c r="E2" s="14">
+        <v>-0.17863299999999999</v>
+      </c>
+      <c r="F2" s="14">
+        <v>0.95182652999999995</v>
+      </c>
+      <c r="G2" s="14">
+        <v>0.81431617000000001</v>
+      </c>
+      <c r="H2" s="14">
+        <v>0.96616599999999997</v>
+      </c>
+      <c r="I2" s="14">
+        <v>1.02581261</v>
+      </c>
+      <c r="J2" s="14">
+        <v>3.41660203</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>14.3</v>
+      </c>
+      <c r="C3" s="14">
+        <v>0.53306534000000005</v>
+      </c>
+      <c r="D3" s="14">
+        <v>1.7798752900000001</v>
+      </c>
+      <c r="E3" s="14">
+        <v>-0.58843800000000002</v>
+      </c>
+      <c r="F3" s="14">
+        <v>0.40988564999999999</v>
+      </c>
+      <c r="G3" s="14">
+        <v>6.6776779999999994E-2</v>
+      </c>
+      <c r="H3" s="14">
+        <v>0.21940499999999999</v>
+      </c>
+      <c r="I3" s="14">
+        <v>0.86898534000000005</v>
+      </c>
+      <c r="J3" s="14">
+        <v>2.5557952099999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="C4" s="14">
+        <v>1.1341932800000001</v>
+      </c>
+      <c r="D4" s="14">
+        <v>1.5759194700000001</v>
+      </c>
+      <c r="E4" s="14">
+        <v>0.57824399999999998</v>
+      </c>
+      <c r="F4" s="14">
+        <v>0.48913411000000001</v>
+      </c>
+      <c r="G4" s="14">
+        <v>0.26875001999999998</v>
+      </c>
+      <c r="H4" s="14">
+        <v>-0.18554000000000001</v>
+      </c>
+      <c r="I4" s="14">
+        <v>1.1794140399999999</v>
+      </c>
+      <c r="J4" s="14">
+        <v>2.2201672100000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>15.9</v>
+      </c>
+      <c r="C5" s="14">
+        <v>0.79184779999999999</v>
+      </c>
+      <c r="D5" s="14">
+        <v>1.5794215</v>
+      </c>
+      <c r="E5" s="14">
+        <v>-7.2789999999999999E-3</v>
+      </c>
+      <c r="F5" s="14">
+        <v>0.98951290000000003</v>
+      </c>
+      <c r="G5" s="14">
+        <v>0.81306818999999997</v>
+      </c>
+      <c r="H5" s="14">
+        <v>0.69578799999999996</v>
+      </c>
+      <c r="I5" s="14">
+        <v>1.0661048</v>
+      </c>
+      <c r="J5" s="14">
+        <v>3.4135301199999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF43263-32D8-3C45-B9C0-C04E7F4D9FE0}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2242,7 +2578,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -2316,12 +2652,231 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08CA3D2A-009B-FE40-89DF-40F277A203D2}">
+  <dimension ref="A1:L5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.83203125" style="21"/>
+    <col min="5" max="5" width="11.5" style="21" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="21"/>
+    <col min="7" max="7" width="11.6640625" style="21" customWidth="1"/>
+    <col min="8" max="10" width="10.83203125" style="21"/>
+    <col min="11" max="11" width="11.33203125" style="21" customWidth="1"/>
+    <col min="12" max="12" width="10.83203125" style="21"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="6">
+        <v>15.9</v>
+      </c>
+      <c r="C2" s="21">
+        <v>-3.2927999999999999E-2</v>
+      </c>
+      <c r="D2" s="21">
+        <v>2.1116790000000001</v>
+      </c>
+      <c r="E2" s="21">
+        <v>-9.1219999999999996E-2</v>
+      </c>
+      <c r="F2" s="21">
+        <v>1.2081170000000001</v>
+      </c>
+      <c r="G2" s="21">
+        <v>-0.26727200000000001</v>
+      </c>
+      <c r="H2" s="21">
+        <v>-2.2743850000000001</v>
+      </c>
+      <c r="I2" s="21">
+        <v>8.8829000000000005E-2</v>
+      </c>
+      <c r="J2" s="21">
+        <v>0</v>
+      </c>
+      <c r="K2" s="21">
+        <v>0.37493900000000002</v>
+      </c>
+      <c r="L2" s="21">
+        <v>1.204615</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="6">
+        <v>14.3</v>
+      </c>
+      <c r="C3" s="21">
+        <v>-3.3211999999999998E-2</v>
+      </c>
+      <c r="D3" s="21">
+        <v>2.3385189999999998</v>
+      </c>
+      <c r="E3" s="21">
+        <v>-2.198E-2</v>
+      </c>
+      <c r="F3" s="21">
+        <v>-0.31351000000000001</v>
+      </c>
+      <c r="G3" s="21">
+        <v>-0.30177100000000001</v>
+      </c>
+      <c r="H3" s="21">
+        <v>-2.3298380000000001</v>
+      </c>
+      <c r="I3" s="21">
+        <v>7.9464999999999994E-2</v>
+      </c>
+      <c r="J3" s="21">
+        <v>0</v>
+      </c>
+      <c r="K3" s="21">
+        <v>0.45260499999999998</v>
+      </c>
+      <c r="L3" s="21">
+        <v>1.1620429999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="6">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="C4" s="21">
+        <v>-1.9186000000000002E-2</v>
+      </c>
+      <c r="D4" s="21">
+        <v>1.8059419999999999</v>
+      </c>
+      <c r="E4" s="21">
+        <v>-5.2107000000000001E-2</v>
+      </c>
+      <c r="F4" s="21">
+        <v>-1.9355850000000001</v>
+      </c>
+      <c r="G4" s="21">
+        <v>-3.7863000000000001E-2</v>
+      </c>
+      <c r="H4" s="21">
+        <v>2.4509470000000002</v>
+      </c>
+      <c r="I4" s="21">
+        <v>6.0879000000000003E-2</v>
+      </c>
+      <c r="J4" s="21">
+        <v>0</v>
+      </c>
+      <c r="K4" s="21">
+        <v>0.28348099999999998</v>
+      </c>
+      <c r="L4" s="21">
+        <v>1.2658579999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="6">
+        <v>15.9</v>
+      </c>
+      <c r="C5" s="21">
+        <v>-4.8936E-2</v>
+      </c>
+      <c r="D5" s="21">
+        <v>2.1119789999999998</v>
+      </c>
+      <c r="E5" s="21">
+        <v>-9.1222999999999999E-2</v>
+      </c>
+      <c r="F5" s="21">
+        <v>1.20733</v>
+      </c>
+      <c r="G5" s="21">
+        <v>-0.26730799999999999</v>
+      </c>
+      <c r="H5" s="21">
+        <v>-2.274041</v>
+      </c>
+      <c r="I5" s="21">
+        <v>0.13195200000000001</v>
+      </c>
+      <c r="J5" s="21">
+        <v>0</v>
+      </c>
+      <c r="K5" s="21">
+        <v>0.374471</v>
+      </c>
+      <c r="L5" s="21">
+        <v>1.203681</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F07D9F88-15BB-7E44-A02C-3321FE5E3C69}">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2331,40 +2886,40 @@
     <col min="3" max="3" width="9.33203125" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" style="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.33203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" style="14" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="D1" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>16</v>
-      </c>
       <c r="F1" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="14" t="s">
         <v>17</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -2450,12 +3005,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FDA1F26-81F4-914D-9042-C84EC2FA5C7C}">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection sqref="A1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2465,39 +3020,39 @@
     <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="D1" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>16</v>
-      </c>
       <c r="F1" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="14" t="s">
         <v>17</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -2587,12 +3142,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AC5FA88-BF56-C34B-9EE3-7E83998CCDD4}">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection sqref="A1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2602,39 +3157,39 @@
     <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="D1" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>16</v>
-      </c>
       <c r="F1" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="14" t="s">
         <v>17</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -2724,12 +3279,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{436344CE-FBA7-FA45-99A0-B52AC1980E06}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2739,39 +3294,39 @@
     <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="D1" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>16</v>
-      </c>
       <c r="F1" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="14" t="s">
         <v>17</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -2861,12 +3416,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F572B592-A878-A74C-81FF-84D0E863DFE0}">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2882,22 +3437,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="14" t="s">
         <v>14</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2905,16 +3460,16 @@
         <v>-1</v>
       </c>
       <c r="D2" s="14">
-        <f>-SQRT(15)/10</f>
-        <v>-0.3872983346207417</v>
+        <f>-1/10</f>
+        <v>-0.1</v>
       </c>
       <c r="E2" s="14">
-        <f>SQRT(2)/2</f>
-        <v>0.70710678118654757</v>
+        <f>SQRT(10)/10</f>
+        <v>0.31622776601683794</v>
       </c>
       <c r="F2" s="14">
-        <f>2*SQRT(15)/15</f>
-        <v>0.51639777949432231</v>
+        <f>2*SQRT(21)/105</f>
+        <v>8.7287156094396953E-2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -2926,20 +3481,20 @@
         <v>-0.57735026918962573</v>
       </c>
       <c r="C3" s="14">
-        <f>-SQRT(3)/3</f>
-        <v>-0.57735026918962573</v>
+        <f>-1/3</f>
+        <v>-0.33333333333333331</v>
       </c>
       <c r="D3" s="14">
-        <f>-2*SQRT(15)/15</f>
-        <v>-0.51639777949432231</v>
+        <f>-2/15</f>
+        <v>-0.13333333333333333</v>
       </c>
       <c r="E3" s="14">
-        <f>SQRT(6)/3</f>
-        <v>0.81649658092772592</v>
+        <f t="shared" ref="E3" si="0">SQRT(30)/15</f>
+        <v>0.36514837167011077</v>
       </c>
       <c r="F3" s="14">
-        <f>SQRT(10)/5</f>
-        <v>0.63245553203367588</v>
+        <f>SQRT(14)/35</f>
+        <v>0.10690449676496976</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -2947,16 +3502,16 @@
         <v>1</v>
       </c>
       <c r="D4" s="14">
-        <f>-SQRT(15)/10</f>
-        <v>-0.3872983346207417</v>
+        <f>-1/10</f>
+        <v>-0.1</v>
       </c>
       <c r="E4" s="14">
-        <f>SQRT(2)/2</f>
-        <v>0.70710678118654757</v>
+        <f>SQRT(10)/10</f>
+        <v>0.31622776601683794</v>
       </c>
       <c r="F4" s="14">
-        <f>2*SQRT(15)/15</f>
-        <v>0.51639777949432231</v>
+        <f>2*SQRT(21)/105</f>
+        <v>8.7287156094396953E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update data "Simulated * beta parameters, TD*.xlsx"
</commit_message>
<xml_diff>
--- a/Data/Simulated Ne beta parameters, TDHF, 2018-09-17.xlsx
+++ b/Data/Simulated Ne beta parameters, TDHF, 2018-09-17.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daehyun/Documents/FERMI 20144077 Ueda/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05157CBA-BD6A-9149-B045-7CDD5B6C42C5}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217C1E6E-ACD7-CE4F-B4A8-E3A884380D23}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38580" yWindow="1520" windowWidth="25560" windowHeight="18880" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38580" yWindow="1520" windowWidth="25560" windowHeight="18880" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="w2w" sheetId="18" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="43">
   <si>
     <t>beta1</t>
   </si>
@@ -153,17 +153,31 @@
   </si>
   <si>
     <t>beta1m3_shift</t>
+  </si>
+  <si>
+    <t>Int_w (W/cm2)</t>
+  </si>
+  <si>
+    <t>Int_2w (W/cm2)</t>
+  </si>
+  <si>
+    <t>Int ratio</t>
+  </si>
+  <si>
+    <t>Ref int ratio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="167" formatCode="0.00000"/>
+    <numFmt numFmtId="172" formatCode="0.000E+00"/>
+    <numFmt numFmtId="173" formatCode="0E+00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -201,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -240,11 +254,32 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="87">
+  <dxfs count="91">
+    <dxf>
+      <numFmt numFmtId="172" formatCode="0.000E+00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="172" formatCode="0.000E+00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="173" formatCode="0E+00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.00000"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="166" formatCode="0.000"/>
     </dxf>
@@ -927,12 +962,6 @@
       <numFmt numFmtId="167" formatCode="0.00000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.00000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="165" formatCode="0.0000"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1028,20 +1057,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{8778010A-3D1F-DF4F-B2BA-4CD89121205F}" name="Table1311" displayName="Table1311" ref="A1:H33" totalsRowShown="0" headerRowDxfId="86" dataDxfId="85">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{8778010A-3D1F-DF4F-B2BA-4CD89121205F}" name="Table1311" displayName="Table1311" ref="A1:H33" totalsRowShown="0" headerRowDxfId="90" dataDxfId="89">
   <autoFilter ref="A1:H33" xr:uid="{EE0BDB9F-493C-9C4A-8003-F22A7669AAA7}"/>
   <sortState ref="A2:H33">
     <sortCondition ref="A1:A33"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{A9C0E41B-1AFE-674C-90E8-D1D179628E58}" name="Target dataset" dataDxfId="84"/>
-    <tableColumn id="2" xr3:uid="{6B63E76C-A142-484A-8040-5F9E2B6ED8BF}" name="Photon (eV)" dataDxfId="83"/>
-    <tableColumn id="3" xr3:uid="{C1A5F614-DF39-FE4D-9C68-CF238B7B1FAB}" name="phi (deg)" dataDxfId="82"/>
-    <tableColumn id="4" xr3:uid="{93222719-EACE-D14D-A23C-A29210E3F88D}" name="beta1" dataDxfId="81"/>
-    <tableColumn id="5" xr3:uid="{55463977-50DC-5543-A800-65678C631CA9}" name="beta2" dataDxfId="80"/>
-    <tableColumn id="6" xr3:uid="{A4D18E31-8E47-7540-BFFA-2FF61FA4E199}" name="beta3" dataDxfId="79"/>
-    <tableColumn id="7" xr3:uid="{3032E9A7-5533-1D49-A217-30EF10E5A58C}" name="beta4" dataDxfId="78"/>
-    <tableColumn id="10" xr3:uid="{1466D1E1-9E6B-F34A-A8D5-24AA1175800D}" name="beta1m3" dataDxfId="77">
+    <tableColumn id="1" xr3:uid="{A9C0E41B-1AFE-674C-90E8-D1D179628E58}" name="Target dataset" dataDxfId="88"/>
+    <tableColumn id="2" xr3:uid="{6B63E76C-A142-484A-8040-5F9E2B6ED8BF}" name="Photon (eV)" dataDxfId="87"/>
+    <tableColumn id="3" xr3:uid="{C1A5F614-DF39-FE4D-9C68-CF238B7B1FAB}" name="phi (deg)" dataDxfId="86"/>
+    <tableColumn id="4" xr3:uid="{93222719-EACE-D14D-A23C-A29210E3F88D}" name="beta1" dataDxfId="85"/>
+    <tableColumn id="5" xr3:uid="{55463977-50DC-5543-A800-65678C631CA9}" name="beta2" dataDxfId="84"/>
+    <tableColumn id="6" xr3:uid="{A4D18E31-8E47-7540-BFFA-2FF61FA4E199}" name="beta3" dataDxfId="83"/>
+    <tableColumn id="7" xr3:uid="{3032E9A7-5533-1D49-A217-30EF10E5A58C}" name="beta4" dataDxfId="82"/>
+    <tableColumn id="10" xr3:uid="{1466D1E1-9E6B-F34A-A8D5-24AA1175800D}" name="beta1m3" dataDxfId="81">
       <calculatedColumnFormula>Table1311[[#This Row],[beta1]]-3/2*Table1311[[#This Row],[beta3]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1055,143 +1084,149 @@
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{B583D4BB-9F96-994C-A314-D7FB7341AA8C}" name="Target dataset"/>
     <tableColumn id="2" xr3:uid="{89667834-04CF-9C4D-9D20-6C00DB34F2BF}" name="Photon (eV)"/>
-    <tableColumn id="15" xr3:uid="{60507A89-BBE8-014A-8D9A-13D578F47D96}" name="beta1_amp" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{7C8D09CD-0B6C-6A41-B1CB-73BD882F1E73}" name="beta1_shift" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{8CCA5178-3667-6640-BC8E-D63DA2EE6D29}" name="beta2" dataDxfId="5"/>
-    <tableColumn id="16" xr3:uid="{485E2375-608B-1A48-96B1-B590DD8C5233}" name="beta3_amp" dataDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{240B768E-BBCE-E944-915A-21D3F550E5B5}" name="beta3_shift" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{DAB6A4F1-E777-2240-BCC5-93E270FEEC6D}" name="beta4" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{8A84BA3D-368F-9D40-B237-2CEAFCB73E75}" name="beta1m3_amp" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{ABBF046B-A08D-394B-BE43-B991E954AD0C}" name="beta1m3_shift" dataDxfId="0"/>
+    <tableColumn id="15" xr3:uid="{60507A89-BBE8-014A-8D9A-13D578F47D96}" name="beta1_amp" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{7C8D09CD-0B6C-6A41-B1CB-73BD882F1E73}" name="beta1_shift" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{8CCA5178-3667-6640-BC8E-D63DA2EE6D29}" name="beta2" dataDxfId="11"/>
+    <tableColumn id="16" xr3:uid="{485E2375-608B-1A48-96B1-B590DD8C5233}" name="beta3_amp" dataDxfId="10"/>
+    <tableColumn id="12" xr3:uid="{240B768E-BBCE-E944-915A-21D3F550E5B5}" name="beta3_shift" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{DAB6A4F1-E777-2240-BCC5-93E270FEEC6D}" name="beta4" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{8A84BA3D-368F-9D40-B237-2CEAFCB73E75}" name="beta1m3_amp" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{ABBF046B-A08D-394B-BE43-B991E954AD0C}" name="beta1m3_shift" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F05A4894-8C70-D642-85C3-3AB7CFBB4F28}" name="Table135" displayName="Table135" ref="A1:E4" totalsRowShown="0" headerRowDxfId="76" dataDxfId="75">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F05A4894-8C70-D642-85C3-3AB7CFBB4F28}" name="Table135" displayName="Table135" ref="A1:E4" totalsRowShown="0" headerRowDxfId="80" dataDxfId="79">
   <autoFilter ref="A1:E4" xr:uid="{53E4CFBE-4728-384F-AC3E-37B66AF4A439}"/>
   <sortState ref="A2:E4">
     <sortCondition ref="A1:A4"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="2" xr3:uid="{BD60D2D9-15A2-F545-AAFF-748850E64446}" name="Photon (eV)" dataDxfId="74"/>
-    <tableColumn id="4" xr3:uid="{28273152-69FC-A241-BCA6-31BCEA8C2BEC}" name="beta1" dataDxfId="73"/>
-    <tableColumn id="5" xr3:uid="{33E9B38C-ACC9-0A49-9295-DACDF599E7FB}" name="beta2" dataDxfId="72"/>
-    <tableColumn id="6" xr3:uid="{407B9B6B-64D4-014F-A379-342916257ADC}" name="beta3" dataDxfId="71"/>
-    <tableColumn id="7" xr3:uid="{8826E549-F298-AB41-856D-6CC97B08EAB8}" name="beta4" dataDxfId="70"/>
+    <tableColumn id="2" xr3:uid="{BD60D2D9-15A2-F545-AAFF-748850E64446}" name="Photon (eV)" dataDxfId="78"/>
+    <tableColumn id="4" xr3:uid="{28273152-69FC-A241-BCA6-31BCEA8C2BEC}" name="beta1" dataDxfId="77"/>
+    <tableColumn id="5" xr3:uid="{33E9B38C-ACC9-0A49-9295-DACDF599E7FB}" name="beta2" dataDxfId="76"/>
+    <tableColumn id="6" xr3:uid="{407B9B6B-64D4-014F-A379-342916257ADC}" name="beta3" dataDxfId="75"/>
+    <tableColumn id="7" xr3:uid="{8826E549-F298-AB41-856D-6CC97B08EAB8}" name="beta4" dataDxfId="74"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{648571DC-0017-F44C-9861-5B63C026D27B}" name="Table1" displayName="Table1" ref="A1:L5" totalsRowShown="0">
-  <autoFilter ref="A1:L5" xr:uid="{A6CF40E6-909C-EF45-94C2-61FE41276FD0}"/>
-  <tableColumns count="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{648571DC-0017-F44C-9861-5B63C026D27B}" name="Table1" displayName="Table1" ref="A1:P5" totalsRowShown="0">
+  <autoFilter ref="A1:P5" xr:uid="{A6CF40E6-909C-EF45-94C2-61FE41276FD0}"/>
+  <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{8EA12F60-3AC0-1B4B-BCF6-65DDE53BE438}" name="Target dataset"/>
-    <tableColumn id="2" xr3:uid="{90E968C9-0904-3A4F-B492-15BEF052B297}" name="Photon (eV)" dataDxfId="69"/>
-    <tableColumn id="3" xr3:uid="{1B597EDE-219E-6241-B37F-8CED0F7B29A1}" name="coeff_sp" dataDxfId="68"/>
-    <tableColumn id="4" xr3:uid="{AA9F4726-D238-224F-9511-86ABE8AC5E51}" name="eta_sp" dataDxfId="67"/>
-    <tableColumn id="5" xr3:uid="{AF5D9ABC-E405-664C-BD87-0CEBF507E41D}" name="coeff_psp" dataDxfId="66"/>
-    <tableColumn id="6" xr3:uid="{64A2F11E-FF0F-A54A-8571-8DCE1875A6D8}" name="eta_psp" dataDxfId="65"/>
-    <tableColumn id="7" xr3:uid="{B475181D-DB43-F347-AC5B-1ADBA027A415}" name="coeff_pdp" dataDxfId="64"/>
-    <tableColumn id="8" xr3:uid="{D74F1B77-0598-E047-BE9E-65FFAA85DFE0}" name="eta_pdp" dataDxfId="63"/>
-    <tableColumn id="9" xr3:uid="{D7428F5C-8F9B-3A4E-BE08-93156A3D8070}" name="coeff_dp" dataDxfId="62"/>
-    <tableColumn id="10" xr3:uid="{219D52DC-F4B2-2846-AE03-BF070C4B6292}" name="eta_dp" dataDxfId="61"/>
-    <tableColumn id="11" xr3:uid="{A8716C4F-8448-6947-98AC-C95A3FA898C7}" name="coeff_fdp" dataDxfId="60"/>
-    <tableColumn id="12" xr3:uid="{C15B8245-F0D7-EB45-8808-6810DC739D05}" name="eta_fdp" dataDxfId="59"/>
+    <tableColumn id="2" xr3:uid="{90E968C9-0904-3A4F-B492-15BEF052B297}" name="Photon (eV)" dataDxfId="4"/>
+    <tableColumn id="16" xr3:uid="{BF5FFC71-AF55-E84A-8E91-9E94DFE7AF9C}" name="Int_w (W/cm2)" dataDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{5EC2CB21-57AD-3E43-AC48-433080EF12C2}" name="Int_2w (W/cm2)" dataDxfId="2"/>
+    <tableColumn id="14" xr3:uid="{ACBEC225-2D80-0C4B-ACE9-6521D6167342}" name="Int ratio" dataDxfId="0">
+      <calculatedColumnFormula>Table1[[#This Row],[Int_2w (W/cm2)]]^0.5/Table1[[#This Row],[Int_w (W/cm2)]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="13" xr3:uid="{4F32759A-5D66-3F48-9F54-BE87A13BF3AC}" name="Ref int ratio" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{1B597EDE-219E-6241-B37F-8CED0F7B29A1}" name="coeff_sp" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{AA9F4726-D238-224F-9511-86ABE8AC5E51}" name="eta_sp" dataDxfId="73"/>
+    <tableColumn id="5" xr3:uid="{AF5D9ABC-E405-664C-BD87-0CEBF507E41D}" name="coeff_psp" dataDxfId="72"/>
+    <tableColumn id="6" xr3:uid="{64A2F11E-FF0F-A54A-8571-8DCE1875A6D8}" name="eta_psp" dataDxfId="71"/>
+    <tableColumn id="7" xr3:uid="{B475181D-DB43-F347-AC5B-1ADBA027A415}" name="coeff_pdp" dataDxfId="70"/>
+    <tableColumn id="8" xr3:uid="{D74F1B77-0598-E047-BE9E-65FFAA85DFE0}" name="eta_pdp" dataDxfId="69"/>
+    <tableColumn id="9" xr3:uid="{D7428F5C-8F9B-3A4E-BE08-93156A3D8070}" name="coeff_dp" dataDxfId="68"/>
+    <tableColumn id="10" xr3:uid="{219D52DC-F4B2-2846-AE03-BF070C4B6292}" name="eta_dp" dataDxfId="67"/>
+    <tableColumn id="11" xr3:uid="{A8716C4F-8448-6947-98AC-C95A3FA898C7}" name="coeff_fdp" dataDxfId="66"/>
+    <tableColumn id="12" xr3:uid="{C15B8245-F0D7-EB45-8808-6810DC739D05}" name="eta_fdp" dataDxfId="65"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{59DFE585-94CE-324E-80C4-17D5A8535F3A}" name="Table3" displayName="Table3" ref="A1:I4" totalsRowShown="0" headerRowDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{59DFE585-94CE-324E-80C4-17D5A8535F3A}" name="Table3" displayName="Table3" ref="A1:I4" totalsRowShown="0" headerRowDxfId="64">
   <autoFilter ref="A1:I4" xr:uid="{8B5C4BC6-D08A-F342-B69E-95E18573CBD5}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{5BA34F36-7497-CA4F-999F-15736C5C90B3}" name="m" dataDxfId="57"/>
-    <tableColumn id="2" xr3:uid="{A0426779-3323-8542-8FAD-30E204B20D55}" name="sp_amp" dataDxfId="56"/>
-    <tableColumn id="3" xr3:uid="{684B6570-B9E4-704D-8176-FCA5A03A637E}" name="p_amp" dataDxfId="55"/>
-    <tableColumn id="4" xr3:uid="{ADC74BA0-1CC4-1C48-A1F6-685EBC267637}" name="dp_amp" dataDxfId="54"/>
-    <tableColumn id="5" xr3:uid="{2845C546-B0B7-214A-9B3A-94C4A1525E23}" name="fdp_amp" dataDxfId="53"/>
-    <tableColumn id="6" xr3:uid="{1E48FDEC-EE5F-7C46-A4AB-BA8213F216B3}" name="sp_shift" dataDxfId="52"/>
-    <tableColumn id="7" xr3:uid="{CD04CD5C-B6F2-9246-BDA1-EA343D3D5323}" name="p_shift" dataDxfId="51"/>
-    <tableColumn id="8" xr3:uid="{9B5BB2F1-9199-A844-952A-2F3D8A2919AF}" name="dp_shift" dataDxfId="50"/>
-    <tableColumn id="9" xr3:uid="{6B1CD9FD-B8D5-2043-9623-1AE12EBE013F}" name="fdp_shift" dataDxfId="49"/>
+    <tableColumn id="1" xr3:uid="{5BA34F36-7497-CA4F-999F-15736C5C90B3}" name="m" dataDxfId="63"/>
+    <tableColumn id="2" xr3:uid="{A0426779-3323-8542-8FAD-30E204B20D55}" name="sp_amp" dataDxfId="62"/>
+    <tableColumn id="3" xr3:uid="{684B6570-B9E4-704D-8176-FCA5A03A637E}" name="p_amp" dataDxfId="61"/>
+    <tableColumn id="4" xr3:uid="{ADC74BA0-1CC4-1C48-A1F6-685EBC267637}" name="dp_amp" dataDxfId="60"/>
+    <tableColumn id="5" xr3:uid="{2845C546-B0B7-214A-9B3A-94C4A1525E23}" name="fdp_amp" dataDxfId="59"/>
+    <tableColumn id="6" xr3:uid="{1E48FDEC-EE5F-7C46-A4AB-BA8213F216B3}" name="sp_shift" dataDxfId="58"/>
+    <tableColumn id="7" xr3:uid="{CD04CD5C-B6F2-9246-BDA1-EA343D3D5323}" name="p_shift" dataDxfId="57"/>
+    <tableColumn id="8" xr3:uid="{9B5BB2F1-9199-A844-952A-2F3D8A2919AF}" name="dp_shift" dataDxfId="56"/>
+    <tableColumn id="9" xr3:uid="{6B1CD9FD-B8D5-2043-9623-1AE12EBE013F}" name="fdp_shift" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{AEAD797E-5610-6742-BF1C-D62A7ADBA7F0}" name="Table5" displayName="Table5" ref="A1:I4" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{AEAD797E-5610-6742-BF1C-D62A7ADBA7F0}" name="Table5" displayName="Table5" ref="A1:I4" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
   <autoFilter ref="A1:I4" xr:uid="{B4719746-BFD9-6D4E-8D94-4B12B338165F}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{647D98FB-251B-4542-BF7C-63F898E9AC7E}" name="m" dataDxfId="46"/>
-    <tableColumn id="2" xr3:uid="{2E22E77A-4173-0D4A-9A6F-7E47D1678087}" name="sp_amp" dataDxfId="45"/>
-    <tableColumn id="3" xr3:uid="{D6903029-EBD1-994F-97CC-EBA1ABF4E926}" name="p_amp" dataDxfId="44"/>
-    <tableColumn id="4" xr3:uid="{3DF53176-C13B-7641-82D5-1BE402BDD02F}" name="dp_amp" dataDxfId="43"/>
-    <tableColumn id="5" xr3:uid="{1060BE76-3E32-1A48-9A41-0593EE6FE8C2}" name="fdp_amp" dataDxfId="42"/>
-    <tableColumn id="6" xr3:uid="{FFBFF49F-1059-1642-8A31-AD573823D3E3}" name="sp_shift" dataDxfId="41"/>
-    <tableColumn id="7" xr3:uid="{1D811937-AFDD-8D48-81C8-B33622C03534}" name="p_shift" dataDxfId="40"/>
-    <tableColumn id="8" xr3:uid="{E126B12C-EED2-324A-A8CC-51A76C96BAAD}" name="dp_shift" dataDxfId="39"/>
-    <tableColumn id="9" xr3:uid="{8C65ED6F-4B8F-3246-ABE2-AE3D22B29FF5}" name="fdp_shift" dataDxfId="38"/>
+    <tableColumn id="1" xr3:uid="{647D98FB-251B-4542-BF7C-63F898E9AC7E}" name="m" dataDxfId="52"/>
+    <tableColumn id="2" xr3:uid="{2E22E77A-4173-0D4A-9A6F-7E47D1678087}" name="sp_amp" dataDxfId="51"/>
+    <tableColumn id="3" xr3:uid="{D6903029-EBD1-994F-97CC-EBA1ABF4E926}" name="p_amp" dataDxfId="50"/>
+    <tableColumn id="4" xr3:uid="{3DF53176-C13B-7641-82D5-1BE402BDD02F}" name="dp_amp" dataDxfId="49"/>
+    <tableColumn id="5" xr3:uid="{1060BE76-3E32-1A48-9A41-0593EE6FE8C2}" name="fdp_amp" dataDxfId="48"/>
+    <tableColumn id="6" xr3:uid="{FFBFF49F-1059-1642-8A31-AD573823D3E3}" name="sp_shift" dataDxfId="47"/>
+    <tableColumn id="7" xr3:uid="{1D811937-AFDD-8D48-81C8-B33622C03534}" name="p_shift" dataDxfId="46"/>
+    <tableColumn id="8" xr3:uid="{E126B12C-EED2-324A-A8CC-51A76C96BAAD}" name="dp_shift" dataDxfId="45"/>
+    <tableColumn id="9" xr3:uid="{8C65ED6F-4B8F-3246-ABE2-AE3D22B29FF5}" name="fdp_shift" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2A026460-1D43-9646-BB18-B4646ACDCF3D}" name="Table6" displayName="Table6" ref="A1:I4" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2A026460-1D43-9646-BB18-B4646ACDCF3D}" name="Table6" displayName="Table6" ref="A1:I4" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
   <autoFilter ref="A1:I4" xr:uid="{A8FC2363-68E6-1D4F-AF75-C41078FEDC29}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{67A1216D-8F66-8F47-9DDF-9779C464E009}" name="m" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{7A921D8C-3F15-E140-B838-5A1204B74685}" name="sp_amp" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{F8CDDF88-4BC2-1D4A-84BD-6353BF4B9E77}" name="p_amp" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{1481DC66-2D0E-E04E-B630-3C7741CE4CD0}" name="dp_amp" dataDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{720417F9-6520-2C47-B50F-B0B73F912EED}" name="fdp_amp" dataDxfId="31"/>
-    <tableColumn id="6" xr3:uid="{826D4DF2-FA71-F24E-8ED5-A415C4A6D02B}" name="sp_shift" dataDxfId="30"/>
-    <tableColumn id="7" xr3:uid="{D5972777-E932-ED4A-8B82-9C8059F7E06E}" name="p_shift" dataDxfId="29"/>
-    <tableColumn id="8" xr3:uid="{8DE1440F-E3A9-014F-BD79-E3166B7C3A72}" name="dp_shift" dataDxfId="28"/>
-    <tableColumn id="9" xr3:uid="{19C76EA3-897A-3148-80AE-374F812A5850}" name="fdp_shift" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{67A1216D-8F66-8F47-9DDF-9779C464E009}" name="m" dataDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{7A921D8C-3F15-E140-B838-5A1204B74685}" name="sp_amp" dataDxfId="40"/>
+    <tableColumn id="3" xr3:uid="{F8CDDF88-4BC2-1D4A-84BD-6353BF4B9E77}" name="p_amp" dataDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{1481DC66-2D0E-E04E-B630-3C7741CE4CD0}" name="dp_amp" dataDxfId="38"/>
+    <tableColumn id="5" xr3:uid="{720417F9-6520-2C47-B50F-B0B73F912EED}" name="fdp_amp" dataDxfId="37"/>
+    <tableColumn id="6" xr3:uid="{826D4DF2-FA71-F24E-8ED5-A415C4A6D02B}" name="sp_shift" dataDxfId="36"/>
+    <tableColumn id="7" xr3:uid="{D5972777-E932-ED4A-8B82-9C8059F7E06E}" name="p_shift" dataDxfId="35"/>
+    <tableColumn id="8" xr3:uid="{8DE1440F-E3A9-014F-BD79-E3166B7C3A72}" name="dp_shift" dataDxfId="34"/>
+    <tableColumn id="9" xr3:uid="{19C76EA3-897A-3148-80AE-374F812A5850}" name="fdp_shift" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{E38178F3-1826-3E4D-BBB2-2C0D6EDAE208}" name="Table7" displayName="Table7" ref="A1:I4" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{E38178F3-1826-3E4D-BBB2-2C0D6EDAE208}" name="Table7" displayName="Table7" ref="A1:I4" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
   <autoFilter ref="A1:I4" xr:uid="{DC15BAF1-E157-5A42-A33B-060096B22C67}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{FDE47AB7-D70F-3145-A921-E12C0BE05C94}" name="m" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{D43E9326-FEAF-EE49-A01C-CC943A2F4B91}" name="sp_amp" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{7BDC518E-90F1-4D47-A627-F285D44C0247}" name="p_amp" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{EC03AEAB-910C-CD4C-A25B-38E5F1590E5A}" name="dp_amp" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{608F44B2-D548-C349-A1C6-FE7BFEDBADE8}" name="fdp_amp" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{7E6BAB65-DA36-BC48-B2EB-1A3CFDB0CC8D}" name="sp_shift" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{45305CC1-A33F-8644-8440-E87A9BA944D8}" name="p_shift" dataDxfId="18"/>
-    <tableColumn id="8" xr3:uid="{A4952650-FD28-5B48-8679-6D186F7D7ED6}" name="dp_shift" dataDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{B0FF8D19-EC72-B44F-88D1-021AB69F405F}" name="fdp_shift" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{FDE47AB7-D70F-3145-A921-E12C0BE05C94}" name="m" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{D43E9326-FEAF-EE49-A01C-CC943A2F4B91}" name="sp_amp" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{7BDC518E-90F1-4D47-A627-F285D44C0247}" name="p_amp" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{EC03AEAB-910C-CD4C-A25B-38E5F1590E5A}" name="dp_amp" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{608F44B2-D548-C349-A1C6-FE7BFEDBADE8}" name="fdp_amp" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{7E6BAB65-DA36-BC48-B2EB-1A3CFDB0CC8D}" name="sp_shift" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{45305CC1-A33F-8644-8440-E87A9BA944D8}" name="p_shift" dataDxfId="24"/>
+    <tableColumn id="8" xr3:uid="{A4952650-FD28-5B48-8679-6D186F7D7ED6}" name="dp_shift" dataDxfId="23"/>
+    <tableColumn id="9" xr3:uid="{B0FF8D19-EC72-B44F-88D1-021AB69F405F}" name="fdp_shift" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{763C1B8E-8E8C-1C43-AF64-24E938897D53}" name="Table19" displayName="Table19" ref="A1:F4" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{763C1B8E-8E8C-1C43-AF64-24E938897D53}" name="Table19" displayName="Table19" ref="A1:F4" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="A1:F4" xr:uid="{B629EAAC-C030-3144-A5C8-EA87A0850D51}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{678C78C9-26BE-E640-8E8C-8BD4C90EA1D8}" name="m" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{F4BE6F06-FE79-854C-A751-08C0116B4DA2}" name="sp_amp" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{5D349974-DB77-004C-A546-3F935BF8CE78}" name="psp_amp" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{914971F8-D9D5-3042-9BBD-39AA14A4A973}" name="pdp_amp" dataDxfId="10">
+    <tableColumn id="1" xr3:uid="{678C78C9-26BE-E640-8E8C-8BD4C90EA1D8}" name="m" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{F4BE6F06-FE79-854C-A751-08C0116B4DA2}" name="sp_amp" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{5D349974-DB77-004C-A546-3F935BF8CE78}" name="psp_amp" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{914971F8-D9D5-3042-9BBD-39AA14A4A973}" name="pdp_amp" dataDxfId="16">
       <calculatedColumnFormula>-SQRT(15)/10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{1E5B610A-F2B0-C845-8B12-F74BAEE6BEAC}" name="dp_amp" dataDxfId="9">
+    <tableColumn id="5" xr3:uid="{1E5B610A-F2B0-C845-8B12-F74BAEE6BEAC}" name="dp_amp" dataDxfId="15">
       <calculatedColumnFormula>SQRT(30)/15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9597E78F-47B1-1F45-BC2F-077AD7E519D2}" name="fdp_amp" dataDxfId="8">
+    <tableColumn id="6" xr3:uid="{9597E78F-47B1-1F45-BC2F-077AD7E519D2}" name="fdp_amp" dataDxfId="14">
       <calculatedColumnFormula>2*SQRT(15)/15</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2379,8 +2414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1CACF38-0506-9A43-8C40-38E5FAC9927C}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2654,212 +2689,280 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08CA3D2A-009B-FE40-89DF-40F277A203D2}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.83203125" style="21"/>
-    <col min="5" max="5" width="11.5" style="21" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="21"/>
-    <col min="7" max="7" width="11.6640625" style="21" customWidth="1"/>
-    <col min="8" max="10" width="10.83203125" style="21"/>
-    <col min="11" max="11" width="11.33203125" style="21" customWidth="1"/>
-    <col min="12" max="12" width="10.83203125" style="21"/>
+    <col min="3" max="3" width="16.83203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" style="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" style="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.83203125" style="21"/>
+    <col min="9" max="9" width="11.5" style="21" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" style="21"/>
+    <col min="11" max="11" width="11.6640625" style="21" customWidth="1"/>
+    <col min="12" max="14" width="10.83203125" style="21"/>
+    <col min="15" max="15" width="11.33203125" style="21" customWidth="1"/>
+    <col min="16" max="16" width="10.83203125" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>31</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="H1" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="I1" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="K1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="L1" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="M1" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="N1" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="O1" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="P1" s="21" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="6">
         <v>15.9</v>
       </c>
-      <c r="C2" s="21">
+      <c r="C2" s="24">
+        <v>10000000000000</v>
+      </c>
+      <c r="D2" s="22">
+        <v>2200000000</v>
+      </c>
+      <c r="E2" s="23">
+        <f>Table1[[#This Row],[Int_2w (W/cm2)]]^0.5/Table1[[#This Row],[Int_w (W/cm2)]]</f>
+        <v>4.6904157598234302E-9</v>
+      </c>
+      <c r="F2" s="23">
+        <v>1.1180339887498947E-8</v>
+      </c>
+      <c r="G2" s="21">
         <v>-3.2927999999999999E-2</v>
       </c>
-      <c r="D2" s="21">
+      <c r="H2" s="21">
         <v>2.1116790000000001</v>
       </c>
-      <c r="E2" s="21">
+      <c r="I2" s="21">
         <v>-9.1219999999999996E-2</v>
       </c>
-      <c r="F2" s="21">
+      <c r="J2" s="21">
         <v>1.2081170000000001</v>
       </c>
-      <c r="G2" s="21">
+      <c r="K2" s="21">
         <v>-0.26727200000000001</v>
       </c>
-      <c r="H2" s="21">
+      <c r="L2" s="21">
         <v>-2.2743850000000001</v>
       </c>
-      <c r="I2" s="21">
+      <c r="M2" s="21">
         <v>8.8829000000000005E-2</v>
       </c>
-      <c r="J2" s="21">
+      <c r="N2" s="21">
         <v>0</v>
       </c>
-      <c r="K2" s="21">
+      <c r="O2" s="21">
         <v>0.37493900000000002</v>
       </c>
-      <c r="L2" s="21">
+      <c r="P2" s="21">
         <v>1.204615</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="6">
         <v>14.3</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="24">
+        <v>10000000000000</v>
+      </c>
+      <c r="D3" s="22">
+        <v>1540000000</v>
+      </c>
+      <c r="E3" s="23">
+        <f>Table1[[#This Row],[Int_2w (W/cm2)]]^0.5/Table1[[#This Row],[Int_w (W/cm2)]]</f>
+        <v>3.924283374069717E-9</v>
+      </c>
+      <c r="F3" s="23">
+        <v>1.1661903789690601E-8</v>
+      </c>
+      <c r="G3" s="21">
         <v>-3.3211999999999998E-2</v>
       </c>
-      <c r="D3" s="21">
+      <c r="H3" s="21">
         <v>2.3385189999999998</v>
       </c>
-      <c r="E3" s="21">
+      <c r="I3" s="21">
         <v>-2.198E-2</v>
       </c>
-      <c r="F3" s="21">
+      <c r="J3" s="21">
         <v>-0.31351000000000001</v>
       </c>
-      <c r="G3" s="21">
+      <c r="K3" s="21">
         <v>-0.30177100000000001</v>
       </c>
-      <c r="H3" s="21">
+      <c r="L3" s="21">
         <v>-2.3298380000000001</v>
       </c>
-      <c r="I3" s="21">
+      <c r="M3" s="21">
         <v>7.9464999999999994E-2</v>
       </c>
-      <c r="J3" s="21">
+      <c r="N3" s="21">
         <v>0</v>
       </c>
-      <c r="K3" s="21">
+      <c r="O3" s="21">
         <v>0.45260499999999998</v>
       </c>
-      <c r="L3" s="21">
+      <c r="P3" s="21">
         <v>1.1620429999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="6">
         <v>19.100000000000001</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="24">
+        <v>10000000000000</v>
+      </c>
+      <c r="D4" s="22">
+        <v>1490000000</v>
+      </c>
+      <c r="E4" s="23">
+        <f>Table1[[#This Row],[Int_2w (W/cm2)]]^0.5/Table1[[#This Row],[Int_w (W/cm2)]]</f>
+        <v>3.8600518131237567E-9</v>
+      </c>
+      <c r="F4" s="23">
+        <v>1.0488088481701517E-8</v>
+      </c>
+      <c r="G4" s="21">
         <v>-1.9186000000000002E-2</v>
       </c>
-      <c r="D4" s="21">
+      <c r="H4" s="21">
         <v>1.8059419999999999</v>
       </c>
-      <c r="E4" s="21">
+      <c r="I4" s="21">
         <v>-5.2107000000000001E-2</v>
       </c>
-      <c r="F4" s="21">
+      <c r="J4" s="21">
         <v>-1.9355850000000001</v>
       </c>
-      <c r="G4" s="21">
+      <c r="K4" s="21">
         <v>-3.7863000000000001E-2</v>
       </c>
-      <c r="H4" s="21">
+      <c r="L4" s="21">
         <v>2.4509470000000002</v>
       </c>
-      <c r="I4" s="21">
+      <c r="M4" s="21">
         <v>6.0879000000000003E-2</v>
       </c>
-      <c r="J4" s="21">
+      <c r="N4" s="21">
         <v>0</v>
       </c>
-      <c r="K4" s="21">
+      <c r="O4" s="21">
         <v>0.28348099999999998</v>
       </c>
-      <c r="L4" s="21">
+      <c r="P4" s="21">
         <v>1.2658579999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="6">
         <v>15.9</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="24">
+        <v>10000000000000</v>
+      </c>
+      <c r="D5" s="22">
+        <v>4870000000</v>
+      </c>
+      <c r="E5" s="23">
+        <f>Table1[[#This Row],[Int_2w (W/cm2)]]^0.5/Table1[[#This Row],[Int_w (W/cm2)]]</f>
+        <v>6.9785385289471608E-9</v>
+      </c>
+      <c r="F5" s="23">
+        <v>1.1180339887498947E-8</v>
+      </c>
+      <c r="G5" s="21">
         <v>-4.8936E-2</v>
       </c>
-      <c r="D5" s="21">
+      <c r="H5" s="21">
         <v>2.1119789999999998</v>
       </c>
-      <c r="E5" s="21">
+      <c r="I5" s="21">
         <v>-9.1222999999999999E-2</v>
       </c>
-      <c r="F5" s="21">
+      <c r="J5" s="21">
         <v>1.20733</v>
       </c>
-      <c r="G5" s="21">
+      <c r="K5" s="21">
         <v>-0.26730799999999999</v>
       </c>
-      <c r="H5" s="21">
+      <c r="L5" s="21">
         <v>-2.274041</v>
       </c>
-      <c r="I5" s="21">
+      <c r="M5" s="21">
         <v>0.13195200000000001</v>
       </c>
-      <c r="J5" s="21">
+      <c r="N5" s="21">
         <v>0</v>
       </c>
-      <c r="K5" s="21">
+      <c r="O5" s="21">
         <v>0.374471</v>
       </c>
-      <c r="L5" s="21">
+      <c r="P5" s="21">
         <v>1.203681</v>
       </c>
     </row>

</xml_diff>